<commit_message>
patient sample IDs updated to new ones
</commit_message>
<xml_diff>
--- a/data/covidlung_metadata.xlsx
+++ b/data/covidlung_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvarani.masarapu/Documents/covid_project/github_code/2_QualityControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvarani.masarapu/Documents/covid_project/github_code/DualSRT_Study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8288D721-07C4-4C4D-901D-805EE32C75E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD4C2E-B0DB-DC45-AC25-D2097C9BE825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" xr2:uid="{E698D00F-377E-FD4B-BA60-3BF24CE117E5}"/>
   </bookViews>
@@ -87,43 +87,43 @@
     <t>sample_id</t>
   </si>
   <si>
-    <t>P1CL B1</t>
-  </si>
-  <si>
-    <t>P1CL C1</t>
-  </si>
-  <si>
-    <t>P2CL A1</t>
-  </si>
-  <si>
-    <t>P2CL B1</t>
-  </si>
-  <si>
-    <t>P2CL C1</t>
-  </si>
-  <si>
-    <t>P3CL A1</t>
-  </si>
-  <si>
-    <t>P3CL B1</t>
-  </si>
-  <si>
-    <t>P3CL C1</t>
-  </si>
-  <si>
-    <t>P3CL D1</t>
-  </si>
-  <si>
-    <t>P4nCL A1</t>
-  </si>
-  <si>
-    <t>P4nCL B1</t>
-  </si>
-  <si>
-    <t>P5nCL A1</t>
-  </si>
-  <si>
-    <t>P5nCL B1</t>
+    <t>1C B1</t>
+  </si>
+  <si>
+    <t>1C C1</t>
+  </si>
+  <si>
+    <t>2C A1</t>
+  </si>
+  <si>
+    <t>2C B1</t>
+  </si>
+  <si>
+    <t>2C C1</t>
+  </si>
+  <si>
+    <t>3C A1</t>
+  </si>
+  <si>
+    <t>3C B1</t>
+  </si>
+  <si>
+    <t>3C C1</t>
+  </si>
+  <si>
+    <t>3C D1</t>
+  </si>
+  <si>
+    <t>4nC A1</t>
+  </si>
+  <si>
+    <t>4nC B1</t>
+  </si>
+  <si>
+    <t>5nC A1</t>
+  </si>
+  <si>
+    <t>5nC B1</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>